<commit_message>
regex to search for ticker in file
</commit_message>
<xml_diff>
--- a/sp500-historical-components-and-changes/output.xlsx
+++ b/sp500-historical-components-and-changes/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yingchen\Documents\GitHub\analyzingalpha\sp500-historical-components-and-changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E531476-4C64-4B2D-A2AF-2E1B8D5DF3B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDDC624-EAB9-4769-B9BF-3E7AACCC366F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="18276" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1429,10 +1429,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="C189" sqref="C189"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="3" max="3" width="28.5234375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5234375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
searched word by word
</commit_message>
<xml_diff>
--- a/sp500-historical-components-and-changes/output.xlsx
+++ b/sp500-historical-components-and-changes/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="363">
   <si>
     <t>type</t>
   </si>
@@ -673,13 +673,16 @@
     <t>HII</t>
   </si>
   <si>
+    <t>BCR</t>
+  </si>
+  <si>
     <t>VRSK</t>
   </si>
   <si>
     <t>JOY</t>
   </si>
   <si>
-    <t>HPE</t>
+    <t>HPQ</t>
   </si>
   <si>
     <t>HCBK</t>
@@ -700,6 +703,9 @@
     <t>SIAL</t>
   </si>
   <si>
+    <t>WSH</t>
+  </si>
+  <si>
     <t>FOSL</t>
   </si>
   <si>
@@ -856,6 +862,9 @@
     <t>TDC</t>
   </si>
   <si>
+    <t>R</t>
+  </si>
+  <si>
     <t>RE</t>
   </si>
   <si>
@@ -890,6 +899,9 @@
   </si>
   <si>
     <t>ALLEwi</t>
+  </si>
+  <si>
+    <t>JCP</t>
   </si>
   <si>
     <t>FB</t>
@@ -2105,6 +2117,9 @@
       <c r="C33" t="s">
         <v>38</v>
       </c>
+      <c r="D33" t="s">
+        <v>219</v>
+      </c>
       <c r="E33" s="2">
         <v>43097</v>
       </c>
@@ -2123,7 +2138,7 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E34" s="2">
         <v>42277</v>
@@ -2143,7 +2158,7 @@
         <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E35" s="2">
         <v>42277</v>
@@ -2163,7 +2178,7 @@
         <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E36" s="2">
         <v>42304</v>
@@ -2183,7 +2198,7 @@
         <v>42</v>
       </c>
       <c r="D37" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E37" s="2">
         <v>42304</v>
@@ -2203,7 +2218,7 @@
         <v>43</v>
       </c>
       <c r="D38" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E38" s="2">
         <v>42310</v>
@@ -2223,7 +2238,7 @@
         <v>43</v>
       </c>
       <c r="D39" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E39" s="2">
         <v>42310</v>
@@ -2243,7 +2258,7 @@
         <v>44</v>
       </c>
       <c r="D40" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E40" s="2">
         <v>42317</v>
@@ -2263,7 +2278,7 @@
         <v>45</v>
       </c>
       <c r="D41" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E41" s="2">
         <v>42317</v>
@@ -2283,7 +2298,7 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E42" s="2">
         <v>42320</v>
@@ -2303,7 +2318,7 @@
         <v>47</v>
       </c>
       <c r="D43" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E43" s="2">
         <v>42320</v>
@@ -2322,6 +2337,9 @@
       <c r="C44" t="s">
         <v>48</v>
       </c>
+      <c r="D44" t="s">
+        <v>229</v>
+      </c>
       <c r="E44" s="2">
         <v>42366</v>
       </c>
@@ -2340,7 +2358,7 @@
         <v>49</v>
       </c>
       <c r="D45" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E45" s="2">
         <v>42366</v>
@@ -2360,7 +2378,7 @@
         <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E46" s="2">
         <v>42382</v>
@@ -2380,7 +2398,7 @@
         <v>51</v>
       </c>
       <c r="D47" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E47" s="2">
         <v>42382</v>
@@ -2400,7 +2418,7 @@
         <v>52</v>
       </c>
       <c r="D48" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E48" s="2">
         <v>42391</v>
@@ -2420,7 +2438,7 @@
         <v>53</v>
       </c>
       <c r="D49" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E49" s="2">
         <v>42391</v>
@@ -2440,7 +2458,7 @@
         <v>54</v>
       </c>
       <c r="D50" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E50" s="2">
         <v>42395</v>
@@ -2460,7 +2478,7 @@
         <v>55</v>
       </c>
       <c r="D51" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E51" s="2">
         <v>42395</v>
@@ -2480,7 +2498,7 @@
         <v>56</v>
       </c>
       <c r="D52" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E52" s="2">
         <v>42416</v>
@@ -2500,7 +2518,7 @@
         <v>57</v>
       </c>
       <c r="D53" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E53" s="2">
         <v>42416</v>
@@ -2520,7 +2538,7 @@
         <v>58</v>
       </c>
       <c r="D54" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E54" s="2">
         <v>42430</v>
@@ -2540,7 +2558,7 @@
         <v>59</v>
       </c>
       <c r="D55" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E55" s="2">
         <v>42430</v>
@@ -2580,7 +2598,7 @@
         <v>61</v>
       </c>
       <c r="D57" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E57" s="2">
         <v>42432</v>
@@ -2600,7 +2618,7 @@
         <v>62</v>
       </c>
       <c r="D58" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E58" s="2">
         <v>42457</v>
@@ -2620,7 +2638,7 @@
         <v>63</v>
       </c>
       <c r="D59" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E59" s="2">
         <v>42457</v>
@@ -2640,7 +2658,7 @@
         <v>64</v>
       </c>
       <c r="D60" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E60" s="2">
         <v>42467</v>
@@ -2660,7 +2678,7 @@
         <v>65</v>
       </c>
       <c r="D61" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E61" s="2">
         <v>42467</v>
@@ -2680,7 +2698,7 @@
         <v>66</v>
       </c>
       <c r="D62" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E62" s="2">
         <v>42479</v>
@@ -2700,7 +2718,7 @@
         <v>67</v>
       </c>
       <c r="D63" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E63" s="2">
         <v>42479</v>
@@ -2720,7 +2738,7 @@
         <v>68</v>
       </c>
       <c r="D64" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E64" s="2">
         <v>42500</v>
@@ -2740,7 +2758,7 @@
         <v>69</v>
       </c>
       <c r="D65" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E65" s="2">
         <v>42500</v>
@@ -2760,7 +2778,7 @@
         <v>70</v>
       </c>
       <c r="D66" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E66" s="2">
         <v>42503</v>
@@ -2780,7 +2798,7 @@
         <v>71</v>
       </c>
       <c r="D67" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E67" s="2">
         <v>42503</v>
@@ -2820,7 +2838,7 @@
         <v>73</v>
       </c>
       <c r="D69" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E69" s="2">
         <v>42508</v>
@@ -2840,7 +2858,7 @@
         <v>74</v>
       </c>
       <c r="D70" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E70" s="2">
         <v>42514</v>
@@ -2860,7 +2878,7 @@
         <v>75</v>
       </c>
       <c r="D71" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E71" s="2">
         <v>42514</v>
@@ -2880,7 +2898,7 @@
         <v>76</v>
       </c>
       <c r="D72" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E72" s="2">
         <v>42542</v>
@@ -2900,7 +2918,7 @@
         <v>77</v>
       </c>
       <c r="D73" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E73" s="2">
         <v>42542</v>
@@ -2920,7 +2938,7 @@
         <v>78</v>
       </c>
       <c r="D74" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E74" s="2">
         <v>42544</v>
@@ -2940,7 +2958,7 @@
         <v>79</v>
       </c>
       <c r="D75" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E75" s="2">
         <v>42544</v>
@@ -2960,7 +2978,7 @@
         <v>80</v>
       </c>
       <c r="D76" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E76" s="2">
         <v>42544</v>
@@ -2980,7 +2998,7 @@
         <v>81</v>
       </c>
       <c r="D77" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E77" s="2">
         <v>42544</v>
@@ -3000,7 +3018,7 @@
         <v>82</v>
       </c>
       <c r="D78" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E78" s="2">
         <v>42550</v>
@@ -3020,7 +3038,7 @@
         <v>83</v>
       </c>
       <c r="D79" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E79" s="2">
         <v>42550</v>
@@ -3040,7 +3058,7 @@
         <v>84</v>
       </c>
       <c r="D80" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E80" s="2">
         <v>42607</v>
@@ -3060,7 +3078,7 @@
         <v>85</v>
       </c>
       <c r="D81" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E81" s="2">
         <v>42607</v>
@@ -3080,7 +3098,7 @@
         <v>86</v>
       </c>
       <c r="D82" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E82" s="2">
         <v>42640</v>
@@ -3100,7 +3118,7 @@
         <v>87</v>
       </c>
       <c r="D83" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E83" s="2">
         <v>42640</v>
@@ -3120,7 +3138,7 @@
         <v>88</v>
       </c>
       <c r="D84" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E84" s="2">
         <v>42738</v>
@@ -3140,7 +3158,7 @@
         <v>89</v>
       </c>
       <c r="D85" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E85" s="2">
         <v>42738</v>
@@ -3160,7 +3178,7 @@
         <v>90</v>
       </c>
       <c r="D86" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E86" s="2">
         <v>42800</v>
@@ -3180,7 +3198,7 @@
         <v>91</v>
       </c>
       <c r="D87" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E87" s="2">
         <v>42800</v>
@@ -3200,7 +3218,7 @@
         <v>92</v>
       </c>
       <c r="D88" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E88" s="2">
         <v>42822</v>
@@ -3220,7 +3238,7 @@
         <v>93</v>
       </c>
       <c r="D89" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E89" s="2">
         <v>42822</v>
@@ -3240,7 +3258,7 @@
         <v>94</v>
       </c>
       <c r="D90" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E90" s="2">
         <v>42823</v>
@@ -3260,7 +3278,7 @@
         <v>95</v>
       </c>
       <c r="D91" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E91" s="2">
         <v>42823</v>
@@ -3280,7 +3298,7 @@
         <v>96</v>
       </c>
       <c r="D92" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E92" s="2">
         <v>42879</v>
@@ -3300,7 +3318,7 @@
         <v>97</v>
       </c>
       <c r="D93" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="E93" s="2">
         <v>42879</v>
@@ -3320,7 +3338,7 @@
         <v>98</v>
       </c>
       <c r="D94" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E94" s="2">
         <v>42895</v>
@@ -3340,7 +3358,7 @@
         <v>99</v>
       </c>
       <c r="D95" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E95" s="2">
         <v>42895</v>
@@ -3360,7 +3378,7 @@
         <v>100</v>
       </c>
       <c r="D96" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E96" s="2">
         <v>42895</v>
@@ -3380,7 +3398,7 @@
         <v>101</v>
       </c>
       <c r="D97" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E97" s="2">
         <v>42895</v>
@@ -3400,7 +3418,7 @@
         <v>102</v>
       </c>
       <c r="D98" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E98" s="2">
         <v>42895</v>
@@ -3419,6 +3437,9 @@
       <c r="C99" t="s">
         <v>103</v>
       </c>
+      <c r="D99" t="s">
+        <v>282</v>
+      </c>
       <c r="E99" s="2">
         <v>42895</v>
       </c>
@@ -3437,7 +3458,7 @@
         <v>104</v>
       </c>
       <c r="D100" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E100" s="2">
         <v>42898</v>
@@ -3457,7 +3478,7 @@
         <v>105</v>
       </c>
       <c r="D101" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E101" s="2">
         <v>42898</v>
@@ -3477,7 +3498,7 @@
         <v>106</v>
       </c>
       <c r="D102" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E102" s="2">
         <v>42947</v>
@@ -3497,7 +3518,7 @@
         <v>107</v>
       </c>
       <c r="D103" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E103" s="2">
         <v>42947</v>
@@ -3517,7 +3538,7 @@
         <v>108</v>
       </c>
       <c r="D104" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E104" s="2">
         <v>42971</v>
@@ -3537,7 +3558,7 @@
         <v>109</v>
       </c>
       <c r="D105" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E105" s="2">
         <v>42971</v>
@@ -3557,7 +3578,7 @@
         <v>110</v>
       </c>
       <c r="D106" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="E106" s="2">
         <v>42971</v>
@@ -3594,7 +3615,7 @@
         <v>112</v>
       </c>
       <c r="D108" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E108" s="2">
         <v>42986</v>
@@ -3614,7 +3635,7 @@
         <v>113</v>
       </c>
       <c r="D109" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E109" s="2">
         <v>42986</v>
@@ -3634,7 +3655,7 @@
         <v>114</v>
       </c>
       <c r="D110" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="E110" s="2">
         <v>43012</v>
@@ -3654,7 +3675,7 @@
         <v>115</v>
       </c>
       <c r="D111" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E111" s="2">
         <v>43012</v>
@@ -3674,7 +3695,7 @@
         <v>116</v>
       </c>
       <c r="D112" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="E112" s="2">
         <v>41600</v>
@@ -3693,6 +3714,9 @@
       <c r="C113" t="s">
         <v>117</v>
       </c>
+      <c r="D113" t="s">
+        <v>295</v>
+      </c>
       <c r="E113" s="2">
         <v>41600</v>
       </c>
@@ -3711,7 +3735,7 @@
         <v>118</v>
       </c>
       <c r="D114" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="E114" s="2">
         <v>41619</v>
@@ -3731,7 +3755,7 @@
         <v>119</v>
       </c>
       <c r="D115" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="E115" s="2">
         <v>41619</v>
@@ -3751,7 +3775,7 @@
         <v>120</v>
       </c>
       <c r="D116" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="E116" s="2">
         <v>41619</v>
@@ -3771,7 +3795,7 @@
         <v>121</v>
       </c>
       <c r="D117" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E117" s="2">
         <v>41619</v>
@@ -3791,7 +3815,7 @@
         <v>122</v>
       </c>
       <c r="D118" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="E118" s="2">
         <v>41619</v>
@@ -3811,7 +3835,7 @@
         <v>123</v>
       </c>
       <c r="D119" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="E119" s="2">
         <v>41619</v>
@@ -3831,7 +3855,7 @@
         <v>124</v>
       </c>
       <c r="D120" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="E120" s="2">
         <v>43161</v>
@@ -3851,7 +3875,7 @@
         <v>125</v>
       </c>
       <c r="D121" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="E121" s="2">
         <v>43161</v>
@@ -3871,7 +3895,7 @@
         <v>126</v>
       </c>
       <c r="D122" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="E122" s="2">
         <v>43168</v>
@@ -3891,7 +3915,7 @@
         <v>127</v>
       </c>
       <c r="D123" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="E123" s="2">
         <v>43168</v>
@@ -3931,7 +3955,7 @@
         <v>128</v>
       </c>
       <c r="D125" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="E125" s="2">
         <v>43168</v>
@@ -3951,7 +3975,7 @@
         <v>129</v>
       </c>
       <c r="D126" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="E126" s="2">
         <v>43168</v>
@@ -3971,7 +3995,7 @@
         <v>130</v>
       </c>
       <c r="D127" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="E127" s="2">
         <v>43168</v>
@@ -3991,7 +4015,7 @@
         <v>131</v>
       </c>
       <c r="D128" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="E128" s="2">
         <v>43245</v>
@@ -4011,7 +4035,7 @@
         <v>132</v>
       </c>
       <c r="D129" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="E129" s="2">
         <v>43245</v>
@@ -4031,7 +4055,7 @@
         <v>133</v>
       </c>
       <c r="D130" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="E130" s="2">
         <v>43255</v>
@@ -4051,7 +4075,7 @@
         <v>134</v>
       </c>
       <c r="D131" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="E131" s="2">
         <v>43255</v>
@@ -4071,7 +4095,7 @@
         <v>135</v>
       </c>
       <c r="D132" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="E132" s="2">
         <v>43259</v>
@@ -4091,7 +4115,7 @@
         <v>136</v>
       </c>
       <c r="D133" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="E133" s="2">
         <v>43259</v>
@@ -4111,7 +4135,7 @@
         <v>137</v>
       </c>
       <c r="D134" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="E134" s="2">
         <v>43259</v>
@@ -4131,7 +4155,7 @@
         <v>138</v>
       </c>
       <c r="D135" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="E135" s="2">
         <v>43259</v>
@@ -4151,7 +4175,7 @@
         <v>139</v>
       </c>
       <c r="D136" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="E136" s="2">
         <v>43266</v>
@@ -4171,7 +4195,7 @@
         <v>140</v>
       </c>
       <c r="D137" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="E137" s="2">
         <v>43266</v>
@@ -4191,7 +4215,7 @@
         <v>141</v>
       </c>
       <c r="D138" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="E138" s="2">
         <v>43276</v>
@@ -4211,7 +4235,7 @@
         <v>142</v>
       </c>
       <c r="D139" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="E139" s="2">
         <v>43276</v>
@@ -4231,7 +4255,7 @@
         <v>143</v>
       </c>
       <c r="D140" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="E140" s="2">
         <v>43335</v>
@@ -4291,7 +4315,7 @@
         <v>145</v>
       </c>
       <c r="D143" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="E143" s="2">
         <v>43354</v>
@@ -4311,7 +4335,7 @@
         <v>146</v>
       </c>
       <c r="D144" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="E144" s="2">
         <v>43368</v>
@@ -4331,7 +4355,7 @@
         <v>147</v>
       </c>
       <c r="D145" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E145" s="2">
         <v>43368</v>
@@ -4351,7 +4375,7 @@
         <v>148</v>
       </c>
       <c r="D146" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="E146" s="2">
         <v>43377</v>
@@ -4371,7 +4395,7 @@
         <v>149</v>
       </c>
       <c r="D147" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="E147" s="2">
         <v>43377</v>
@@ -4391,7 +4415,7 @@
         <v>150</v>
       </c>
       <c r="D148" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="E148" s="2">
         <v>43403</v>
@@ -4431,7 +4455,7 @@
         <v>152</v>
       </c>
       <c r="D150" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E150" s="2">
         <v>43411</v>
@@ -4471,7 +4495,7 @@
         <v>154</v>
       </c>
       <c r="D152" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="E152" s="2">
         <v>43430</v>
@@ -4491,7 +4515,7 @@
         <v>155</v>
       </c>
       <c r="D153" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="E153" s="2">
         <v>43430</v>
@@ -4511,7 +4535,7 @@
         <v>156</v>
       </c>
       <c r="D154" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="E154" s="2">
         <v>43430</v>
@@ -4531,7 +4555,7 @@
         <v>157</v>
       </c>
       <c r="D155" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="E155" s="2">
         <v>43430</v>
@@ -4551,7 +4575,7 @@
         <v>158</v>
       </c>
       <c r="D156" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="E156" s="2">
         <v>43430</v>
@@ -4571,7 +4595,7 @@
         <v>159</v>
       </c>
       <c r="D157" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="E157" s="2">
         <v>43430</v>
@@ -4591,7 +4615,7 @@
         <v>160</v>
       </c>
       <c r="D158" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="E158" s="2">
         <v>43453</v>
@@ -4611,7 +4635,7 @@
         <v>161</v>
       </c>
       <c r="D159" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="E159" s="2">
         <v>43453</v>
@@ -4631,7 +4655,7 @@
         <v>162</v>
       </c>
       <c r="D160" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="E160" s="2">
         <v>43461</v>
@@ -4651,7 +4675,7 @@
         <v>163</v>
       </c>
       <c r="D161" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="E161" s="2">
         <v>43461</v>
@@ -4671,7 +4695,7 @@
         <v>164</v>
       </c>
       <c r="D162" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="E162" s="2">
         <v>43480</v>
@@ -4691,7 +4715,7 @@
         <v>165</v>
       </c>
       <c r="D163" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="E163" s="2">
         <v>43480</v>
@@ -4711,7 +4735,7 @@
         <v>166</v>
       </c>
       <c r="D164" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E164" s="2">
         <v>43504</v>
@@ -4731,7 +4755,7 @@
         <v>167</v>
       </c>
       <c r="D165" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="E165" s="2">
         <v>43504</v>
@@ -4751,7 +4775,7 @@
         <v>168</v>
       </c>
       <c r="D166" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="E166" s="2">
         <v>43517</v>
@@ -4771,7 +4795,7 @@
         <v>169</v>
       </c>
       <c r="D167" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="E167" s="2">
         <v>43517</v>
@@ -4825,7 +4849,7 @@
         <v>172</v>
       </c>
       <c r="D170" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="E170" s="2">
         <v>43550</v>
@@ -4845,7 +4869,7 @@
         <v>106</v>
       </c>
       <c r="D171" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E171" s="2">
         <v>43550</v>
@@ -4865,7 +4889,7 @@
         <v>173</v>
       </c>
       <c r="D172" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="E172" s="2">
         <v>43613</v>
@@ -4885,7 +4909,7 @@
         <v>174</v>
       </c>
       <c r="D173" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="E173" s="2">
         <v>43613</v>
@@ -4905,7 +4929,7 @@
         <v>175</v>
       </c>
       <c r="D174" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="E174" s="2">
         <v>43619</v>
@@ -4925,7 +4949,7 @@
         <v>176</v>
       </c>
       <c r="D175" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="E175" s="2">
         <v>43619</v>
@@ -4945,7 +4969,7 @@
         <v>177</v>
       </c>
       <c r="D176" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="E176" s="2">
         <v>43640</v>
@@ -4965,7 +4989,7 @@
         <v>178</v>
       </c>
       <c r="D177" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="E177" s="2">
         <v>43640</v>
@@ -4985,7 +5009,7 @@
         <v>179</v>
       </c>
       <c r="D178" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="E178" s="2">
         <v>43655</v>
@@ -5005,7 +5029,7 @@
         <v>180</v>
       </c>
       <c r="D179" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="E179" s="2">
         <v>43655</v>
@@ -5025,7 +5049,7 @@
         <v>181</v>
       </c>
       <c r="D180" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="E180" s="2">
         <v>43678</v>
@@ -5045,7 +5069,7 @@
         <v>182</v>
       </c>
       <c r="D181" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="E181" s="2">
         <v>43678</v>
@@ -5065,7 +5089,7 @@
         <v>183</v>
       </c>
       <c r="D182" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="E182" s="2">
         <v>43678</v>
@@ -5085,7 +5109,7 @@
         <v>62</v>
       </c>
       <c r="D183" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E183" s="2">
         <v>43678</v>
@@ -5105,7 +5129,7 @@
         <v>184</v>
       </c>
       <c r="D184" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="E184" s="2">
         <v>41528</v>
@@ -5125,7 +5149,7 @@
         <v>185</v>
       </c>
       <c r="D185" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="E185" s="2">
         <v>41528</v>
@@ -5145,7 +5169,7 @@
         <v>186</v>
       </c>
       <c r="D186" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="E186" s="2">
         <v>41528</v>
@@ -5165,7 +5189,7 @@
         <v>187</v>
       </c>
       <c r="D187" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="E187" s="2">
         <v>41528</v>
@@ -5185,7 +5209,7 @@
         <v>143</v>
       </c>
       <c r="D188" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="E188" s="2">
         <v>43335</v>
@@ -5225,7 +5249,7 @@
         <v>188</v>
       </c>
       <c r="D190" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="E190" s="2">
         <v>41263</v>
@@ -5245,7 +5269,7 @@
         <v>189</v>
       </c>
       <c r="D191" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="E191" s="2">
         <v>41263</v>

</xml_diff>

<commit_message>
included ; in regex
</commit_message>
<xml_diff>
--- a/sp500-historical-components-and-changes/output.xlsx
+++ b/sp500-historical-components-and-changes/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="365">
   <si>
     <t>type</t>
   </si>
@@ -1049,6 +1049,12 @@
   </si>
   <si>
     <t>GT</t>
+  </si>
+  <si>
+    <t>FOXAV;FOXBV</t>
+  </si>
+  <si>
+    <t>FOXA;FOX</t>
   </si>
   <si>
     <t>DOW</t>
@@ -4814,6 +4820,9 @@
       <c r="C168" t="s">
         <v>170</v>
       </c>
+      <c r="D168" t="s">
+        <v>345</v>
+      </c>
       <c r="E168" s="2">
         <v>43538</v>
       </c>
@@ -4831,6 +4840,9 @@
       <c r="C169" t="s">
         <v>171</v>
       </c>
+      <c r="D169" t="s">
+        <v>346</v>
+      </c>
       <c r="E169" s="2">
         <v>43538</v>
       </c>
@@ -4849,7 +4861,7 @@
         <v>172</v>
       </c>
       <c r="D170" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E170" s="2">
         <v>43550</v>
@@ -4889,7 +4901,7 @@
         <v>173</v>
       </c>
       <c r="D172" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E172" s="2">
         <v>43613</v>
@@ -4909,7 +4921,7 @@
         <v>174</v>
       </c>
       <c r="D173" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E173" s="2">
         <v>43613</v>
@@ -4929,7 +4941,7 @@
         <v>175</v>
       </c>
       <c r="D174" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E174" s="2">
         <v>43619</v>
@@ -4949,7 +4961,7 @@
         <v>176</v>
       </c>
       <c r="D175" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E175" s="2">
         <v>43619</v>
@@ -4969,7 +4981,7 @@
         <v>177</v>
       </c>
       <c r="D176" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E176" s="2">
         <v>43640</v>
@@ -4989,7 +5001,7 @@
         <v>178</v>
       </c>
       <c r="D177" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E177" s="2">
         <v>43640</v>
@@ -5009,7 +5021,7 @@
         <v>179</v>
       </c>
       <c r="D178" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E178" s="2">
         <v>43655</v>
@@ -5029,7 +5041,7 @@
         <v>180</v>
       </c>
       <c r="D179" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E179" s="2">
         <v>43655</v>
@@ -5049,7 +5061,7 @@
         <v>181</v>
       </c>
       <c r="D180" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E180" s="2">
         <v>43678</v>
@@ -5069,7 +5081,7 @@
         <v>182</v>
       </c>
       <c r="D181" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E181" s="2">
         <v>43678</v>
@@ -5089,7 +5101,7 @@
         <v>183</v>
       </c>
       <c r="D182" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E182" s="2">
         <v>43678</v>
@@ -5129,7 +5141,7 @@
         <v>184</v>
       </c>
       <c r="D184" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E184" s="2">
         <v>41528</v>
@@ -5149,7 +5161,7 @@
         <v>185</v>
       </c>
       <c r="D185" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E185" s="2">
         <v>41528</v>
@@ -5169,7 +5181,7 @@
         <v>186</v>
       </c>
       <c r="D186" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E186" s="2">
         <v>41528</v>
@@ -5189,7 +5201,7 @@
         <v>187</v>
       </c>
       <c r="D187" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E187" s="2">
         <v>41528</v>
@@ -5249,7 +5261,7 @@
         <v>188</v>
       </c>
       <c r="D190" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E190" s="2">
         <v>41263</v>
@@ -5269,7 +5281,7 @@
         <v>189</v>
       </c>
       <c r="D191" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="E191" s="2">
         <v>41263</v>

</xml_diff>

<commit_message>
cleaned up and renamed
</commit_message>
<xml_diff>
--- a/sp500-historical-components-and-changes/output.xlsx
+++ b/sp500-historical-components-and-changes/output.xlsx
@@ -1,15 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yingchen\Documents\GitHub\analyzingalpha\sp500-historical-components-and-changes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D95DFC6-2096-49D0-8C0F-1684559D2710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18276" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$191</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1105,11 +1114,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1173,6 +1182,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1219,7 +1236,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1251,9 +1268,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1285,6 +1320,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1460,14 +1513,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="28.5234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5234375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1484,7 +1545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1504,7 +1565,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1524,7 +1585,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1544,7 +1605,7 @@
         <v>43741</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1564,7 +1625,7 @@
         <v>43741</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1584,7 +1645,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1604,7 +1665,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1624,7 +1685,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1644,7 +1705,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1664,7 +1725,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1684,7 +1745,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1704,7 +1765,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1724,7 +1785,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1744,7 +1805,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1764,7 +1825,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1784,7 +1845,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1804,7 +1865,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1824,7 +1885,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1844,7 +1905,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1864,7 +1925,7 @@
         <v>43924</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1884,7 +1945,7 @@
         <v>43924</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1904,7 +1965,7 @@
         <v>43927</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1924,7 +1985,7 @@
         <v>43927</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1944,7 +2005,7 @@
         <v>41402</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1964,7 +2025,7 @@
         <v>41402</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1984,7 +2045,7 @@
         <v>41417</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2004,7 +2065,7 @@
         <v>41417</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2024,7 +2085,7 @@
         <v>42074</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2044,7 +2105,7 @@
         <v>42074</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2064,7 +2125,7 @@
         <v>42166</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2084,7 +2145,7 @@
         <v>42166</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2104,7 +2165,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2124,7 +2185,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2144,7 +2205,7 @@
         <v>42284</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2164,7 +2225,7 @@
         <v>42284</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2184,7 +2245,7 @@
         <v>42307</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2204,7 +2265,7 @@
         <v>42310</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2224,7 +2285,7 @@
         <v>42317</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2244,7 +2305,7 @@
         <v>42318</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2264,7 +2325,7 @@
         <v>42325</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2284,7 +2345,7 @@
         <v>42325</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2304,7 +2365,7 @@
         <v>42326</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2324,7 +2385,7 @@
         <v>42326</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2344,7 +2405,7 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2364,7 +2425,7 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2384,7 +2445,7 @@
         <v>42384</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2404,7 +2465,7 @@
         <v>42384</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2424,7 +2485,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2444,7 +2505,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2464,7 +2525,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2484,7 +2545,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2504,7 +2565,7 @@
         <v>42419</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2524,7 +2585,7 @@
         <v>42419</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2544,7 +2605,7 @@
         <v>42432</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2564,7 +2625,7 @@
         <v>42432</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2584,7 +2645,7 @@
         <v>42433</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2604,7 +2665,7 @@
         <v>42433</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2624,7 +2685,7 @@
         <v>42461</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2644,7 +2705,7 @@
         <v>42461</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2664,7 +2725,7 @@
         <v>42475</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2684,7 +2745,7 @@
         <v>42475</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2704,7 +2765,7 @@
         <v>42482</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2724,7 +2785,7 @@
         <v>42482</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2744,7 +2805,7 @@
         <v>42502</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2764,7 +2825,7 @@
         <v>42502</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2784,7 +2845,7 @@
         <v>42507</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2804,7 +2865,7 @@
         <v>42507</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2824,7 +2885,7 @@
         <v>42510</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2844,7 +2905,7 @@
         <v>42510</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2864,7 +2925,7 @@
         <v>42517</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2884,7 +2945,7 @@
         <v>42517</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2904,7 +2965,7 @@
         <v>42544</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2924,7 +2985,7 @@
         <v>42544</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2944,7 +3005,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2964,7 +3025,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2984,7 +3045,7 @@
         <v>42552</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3004,7 +3065,7 @@
         <v>42556</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3024,7 +3085,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3044,7 +3105,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3064,7 +3125,7 @@
         <v>42615</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3084,7 +3145,7 @@
         <v>42615</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3104,7 +3165,7 @@
         <v>42643</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3124,7 +3185,7 @@
         <v>42643</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3144,7 +3205,7 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3164,7 +3225,7 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3184,7 +3245,7 @@
         <v>42807</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3204,7 +3265,7 @@
         <v>42807</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3224,7 +3285,7 @@
         <v>42829</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3244,7 +3305,7 @@
         <v>42829</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3264,7 +3325,7 @@
         <v>42830</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3284,7 +3345,7 @@
         <v>42830</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3304,7 +3365,7 @@
         <v>42888</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3324,7 +3385,7 @@
         <v>42888</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3344,7 +3405,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3364,7 +3425,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3384,7 +3445,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3404,7 +3465,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3424,7 +3485,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3444,7 +3505,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3464,7 +3525,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3484,7 +3545,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3504,7 +3565,7 @@
         <v>42954</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3524,7 +3585,7 @@
         <v>42955</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3544,7 +3605,7 @@
         <v>42976</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3564,7 +3625,7 @@
         <v>42976</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3584,7 +3645,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3604,7 +3665,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3624,7 +3685,7 @@
         <v>42996</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3644,7 +3705,7 @@
         <v>42996</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3664,7 +3725,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3684,7 +3745,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3704,7 +3765,7 @@
         <v>41607</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -3724,7 +3785,7 @@
         <v>41607</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3744,7 +3805,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3764,7 +3825,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3784,7 +3845,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -3804,7 +3865,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -3824,7 +3885,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -3844,7 +3905,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -3864,7 +3925,7 @@
         <v>43166</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3884,7 +3945,7 @@
         <v>43166</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3904,7 +3965,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -3924,7 +3985,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -3944,7 +4005,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -3964,7 +4025,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3984,7 +4045,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -4004,7 +4065,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -4024,7 +4085,7 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -4044,7 +4105,7 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -4064,7 +4125,7 @@
         <v>43258</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -4084,7 +4145,7 @@
         <v>43258</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -4104,7 +4165,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -4124,7 +4185,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -4144,7 +4205,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -4164,7 +4225,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -4184,7 +4245,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -4204,7 +4265,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -4224,7 +4285,7 @@
         <v>43283</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -4244,7 +4305,7 @@
         <v>43283</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -4264,7 +4325,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -4284,7 +4345,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -4304,7 +4365,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -4324,7 +4385,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -4344,7 +4405,7 @@
         <v>43374</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -4364,7 +4425,7 @@
         <v>43374</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -4384,7 +4445,7 @@
         <v>43384</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -4404,7 +4465,7 @@
         <v>43384</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -4424,7 +4485,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -4444,7 +4505,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -4464,7 +4525,7 @@
         <v>43417</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -4484,7 +4545,7 @@
         <v>43417</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -4504,7 +4565,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -4524,7 +4585,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -4544,7 +4605,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -4564,7 +4625,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -4584,7 +4645,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -4604,7 +4665,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -4624,7 +4685,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -4644,7 +4705,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -4664,7 +4725,7 @@
         <v>43467</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -4684,7 +4745,7 @@
         <v>43467</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -4704,7 +4765,7 @@
         <v>43483</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -4724,7 +4785,7 @@
         <v>43483</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -4744,7 +4805,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -4764,7 +4825,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -4784,7 +4845,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -4804,7 +4865,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -4824,7 +4885,7 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -4844,7 +4905,7 @@
         <v>43544</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -4864,7 +4925,7 @@
         <v>43557</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -4884,7 +4945,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -4904,7 +4965,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -4924,7 +4985,7 @@
         <v>43620</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -4944,7 +5005,7 @@
         <v>43623</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -4964,7 +5025,7 @@
         <v>43623</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -4984,7 +5045,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -5004,7 +5065,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -5024,7 +5085,7 @@
         <v>43661</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -5044,7 +5105,7 @@
         <v>43661</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -5064,7 +5125,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -5084,7 +5145,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -5104,7 +5165,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -5124,7 +5185,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -5144,7 +5205,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -5164,7 +5225,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -5184,7 +5245,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -5204,7 +5265,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -5224,7 +5285,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -5244,7 +5305,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -5264,7 +5325,7 @@
         <v>41274</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -5285,6 +5346,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F191" xr:uid="{645281BE-6F57-48D4-8448-7AB2FAA77694}">
+    <filterColumn colId="4">
+      <filters>
+        <dateGroupItem year="2015" dateTimeGrouping="year"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>